<commit_message>
Updated dialogs with libras videos paths
</commit_message>
<xml_diff>
--- a/translation-project/Assets/VIDE/Resources/populate_videos/debug_tables/M010_Mentor0_Dialogue1.json.xlsx
+++ b/translation-project/Assets/VIDE/Resources/populate_videos/debug_tables/M010_Mentor0_Dialogue1.json.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -374,20 +374,25 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>DialogPosition</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Dialogs</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>ClosestDialog</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>ClosestDialogCoord</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>LibrasVideoPath</t>
         </is>
@@ -396,196 +401,231 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ei! Estou vendo você aí, caminhando devagar e olhando para o chão...está interessada em conhecer a vegetação antártica? Lá vai uma dica: nem tudo que é verde é planta! Hehehe. +</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ei! Estou vendo você ai, caminhando devagar e olhando para o chão...está interessada em conhecer a vegetação Antártica? Lá vai uma dica: Nem tudo que é verde é planta! Hehehe. </t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>vegetacao/Bia/B3.vp8</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Eu vou adorar, mas antes você poderia me falar um pouco mais sobre as plantas que existem aqui? +</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Eu vou adorar, mas antes você poderia me falar um pouco mais sobre as plantas que existem aqui? </t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>E3</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>vegetacao/Bia/E3.vp8</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Muito obrigada, agora vou procurar saber como posso ajudar na pesquisa aqui!+</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Muito obrigada, agora vou procurar saber como posso ajudar na pesquisa aqui!</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>H3</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>vegetacao/Bia/H3.vp8</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Entre os grupos de plantas existentes, aqui na Antártica você pode encontrar dois deles: briófitas e angiospermas. Mas fique de olho também nas algas, líquens e cianobactérias, que apesar de não serem plantas, compartilham várias características delas e são encontrados aos montes aqui. Que tal olhar este esquema para saber mais sobre os grupos de plantas?+</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Entre os grupos de plantas existentes, aqui na Antártica você pode encontrar dois deles: briófitas e angiospermas. Mas fique de olho também nas algas, líquens e cianobactérias, que apesar de não serem plantas, compartilham várias características delas e  são encontrados aos montes aqui. Que tal olhar este esquema para saber mais sobre os grupos de plantas?</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>F3</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>vegetacao/Bia/F3.vp8</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ah! Estou mesmo querendo conhecer as plantas do continente gelado! Pode me dar mais dicas?+</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Ah! Estou mesmo querendo conhecer as plantas do continente gelado! Pode me dar mais dicas?</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>vegetacao/Bia/C3.vp8</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
         <is>
           <t xml:space="preserve">Poxa! Que legal! Sabe que as plantas não são chamativas para a maioria dos visitantes da Antártica? Talvez você possa se interessar também em ajudar a pesquisa que estamos fazendo aqui. </t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>Poxa! Que legal! Sabe que as plantas não são chamativas para a maioria dos visitantes da Antártica? Talvez você possa se interessar também em ajudar a pesquisa que estamos fazendo aqui.</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>D3</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>vegetacao/Bia/D3.vp8</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Ei! Estou vendo você aí, caminhando devagar e olhando para o chão...está interessada em conhecer a vegetação antártica? Lá vai uma dica: nem tudo que é verde é planta! Hehehe. -</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Ei! Estou vendo você ai, caminhando devagar e olhando para o chão...está interessada em conhecer a vegetação Antártica? Lá vai uma dica: Nem tudo que é verde é planta! Hehehe. </t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>B3</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>vegetacao/Bia/B3.vp8</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Entre os grupos de plantas existentes, aqui na Antártica você pode encontrar dois deles: briófitas e angiospermas. Mas fique de olho também nas algas, líquens e cianobactérias, que apesar de não serem plantas, compartilham várias características delas e são encontrados aos montes aqui. Que tal olhar este esquema para saber mais sobre os grupos de plantas?-</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Entre os grupos de plantas existentes, aqui na Antártica você pode encontrar dois deles: briófitas e angiospermas. Mas fique de olho também nas algas, líquens e cianobactérias, que apesar de não serem plantas, compartilham várias características delas e  são encontrados aos montes aqui. Que tal olhar este esquema para saber mais sobre os grupos de plantas?</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>F3</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>vegetacao/Bia/F3.vp8</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Eu vou adorar, mas antes você poderia me falar um pouco mais sobre as plantas que existem aqui? -</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Eu vou adorar, mas antes você poderia me falar um pouco mais sobre as plantas que existem aqui? </t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>E3</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>vegetacao/Bia/E3.vp8</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+    <row r="8">
+      <c r="A8" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
         <is>
           <t xml:space="preserve">Vai ser fácil, procure os naturalistas no acampamento! </t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>Vai ser fácil, procure os naturalistas no acampamento!</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>I3</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>vegetacao/Bia/I3.vp8</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Muito obrigada, agora vou procurar saber como posso ajudar na pesquisa aqui!-</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Muito obrigada, agora vou procurar saber como posso ajudar na pesquisa aqui!</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>H3</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>vegetacao/Bia/H3.vp8</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Ah! Estou mesmo querendo conhecer as plantas do continente gelado! Pode me dar mais dicas?-</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Ah! Estou mesmo querendo conhecer as plantas do continente gelado! Pode me dar mais dicas?</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>C3</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>vegetacao/Bia/C3.vp8</t>
         </is>
       </c>
     </row>

</xml_diff>